<commit_message>
More Computing Questions (only slightly)
</commit_message>
<xml_diff>
--- a/Tools/Excel Management System/output.xlsx
+++ b/Tools/Excel Management System/output.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12250" uniqueCount="1635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12275" uniqueCount="1650">
   <si>
     <t>Subject</t>
   </si>
@@ -4934,7 +4934,52 @@
     <t>State a reason why a company may wish to choose a NoSQL DBMS</t>
   </si>
   <si>
-    <t>Extra data requirements not clear or consistent/Flexibility - new fields and be easily added without making changes to existing schema/Ease of accessto all data stored about a single apartment|Better performance speed for simple queries</t>
+    <t>Extra data requirements not clear or consistent/Flexibility - new fields and be easily added without making changes to existing schema/Ease of accessto all data stored about a single apartment/Better performance speed for simple queries</t>
+  </si>
+  <si>
+    <t>There is an address field in this database. Explain why storing this address as a single field is not good database design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An address consists of several components like Postal Code, State, and Street name. It is thus not feasible to validate the full address. Instead, splitting the address into say two fields, address and postal code, allows the database to look up a list of postal codes to validate the new address entered. </t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Give two advantages of packet switching over circuit switching</t>
+  </si>
+  <si>
+    <t>ANY TWO|Packets are rerouted in case of any problems (eg. busy links or disabled links). This ensures reliable communication |It is more efficient for data transmission as it does not require path to be established between the sender and receiver and data are transmitted immediately |Many users can share the same channel simultaneously. Hence packet switching makes use of the band width efficiently</t>
+  </si>
+  <si>
+    <t>Explain why asynchronous data transmission affects network performance</t>
+  </si>
+  <si>
+    <t>Asynchronous transmission is relatively slow due to the additional start and stop bits and gaps between bytes.| These overhead results in more data that needs to be transmitted in the network affecting network performance</t>
+  </si>
+  <si>
+    <t>Describe one benefit of a client-server network over a peer-to-peer network</t>
+  </si>
+  <si>
+    <t>Client-server network is more secured as it contains a list of usernames and passwords for authentication. As all of the information is stored on a server, it is easier to secure data and setting of permissions on the server. |On a peer-to-peer network, data can be distributed across many computers that is acting as both a client and a server. it is much harder to ensure data security across many computers.</t>
+  </si>
+  <si>
+    <t>Give two advantages in storing shared data on a client server network rather than a peer-to-peer network</t>
+  </si>
+  <si>
+    <t>ANY TWO|Client-server has centralised management of the shared data resulting in better security as it can determine who have access rights and what kind for the shared data|Because it is a centralised system, it can be easy to add more resources and clients|Resources of P2P are divided between local activities and servicing network requests from other peers while in a client-server network, each peer has only to service local processing demands while requests for data are rooted to a dedicated server</t>
+  </si>
+  <si>
+    <t>Describe one drawback of a client-server network comparent to a peer-to-peer network</t>
+  </si>
+  <si>
+    <t>Client-server network is more expensive to implement. it usually requires faster and more reliable and robust hardware that costs more. Specialised software like network operating system and systems administrator to configure and oversee the network are other costs incurred that is not incurred on a peer to peer network.|OR|Failure of the server on a client-server network will cripple the whole network. Resources will not be accessible during the downtime and work cannot be done. Unlike a peer to peer where a single failure does not affect all computers.</t>
+  </si>
+  <si>
+    <t>Name three types of component that the booking form could use and dive into the types of data it is used to capture.</t>
+  </si>
+  <si>
+    <t>Radio buttons: Limited multiple choice options to choose from, such as the Vehicle Type (with 3 available options), makes input easy|Text boxes/ Text areas: Open-ended input for the management to type out names, address, and other information that cannot be validated automatically|Data-time input functions/ areas: Areas of the form that can input dates which can be easily standardised and formatted, allows for automatic computation of wire length and costs incurred</t>
   </si>
   <si>
     <t>25m</t>
@@ -4950,7 +4995,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -5015,11 +5060,16 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
     <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Docs-Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -5062,7 +5112,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -5129,10 +5179,13 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -79493,7 +79546,7 @@
       <c r="C3" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="20">
         <v>2.0</v>
       </c>
       <c r="E3" s="20" t="s">
@@ -79522,7 +79575,7 @@
       <c r="C4" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="20">
         <v>3.0</v>
       </c>
       <c r="E4" s="20" t="s">
@@ -79551,7 +79604,7 @@
       <c r="C5" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="20">
         <v>4.0</v>
       </c>
       <c r="E5" s="20" t="s">
@@ -79580,7 +79633,7 @@
       <c r="C6" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="20">
         <v>5.0</v>
       </c>
       <c r="E6" s="20" t="s">
@@ -79609,7 +79662,7 @@
       <c r="C7" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="20">
         <v>6.0</v>
       </c>
       <c r="E7" s="20" t="s">
@@ -79638,7 +79691,7 @@
       <c r="C8" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="20">
         <v>7.0</v>
       </c>
       <c r="E8" s="20" t="s">
@@ -79667,7 +79720,7 @@
       <c r="C9" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="20">
         <v>8.0</v>
       </c>
       <c r="E9" s="20" t="s">
@@ -79696,7 +79749,7 @@
       <c r="C10" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="20">
         <v>9.0</v>
       </c>
       <c r="E10" s="20" t="s">
@@ -79725,7 +79778,7 @@
       <c r="C11" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="20">
         <v>10.0</v>
       </c>
       <c r="E11" s="20" t="s">
@@ -79754,7 +79807,7 @@
       <c r="C12" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="20">
         <v>11.0</v>
       </c>
       <c r="E12" s="20" t="s">
@@ -79783,7 +79836,7 @@
       <c r="C13" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="20">
         <v>12.0</v>
       </c>
       <c r="E13" s="20" t="s">
@@ -79803,25 +79856,25 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="20" t="s">
         <v>1562</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="20">
         <v>13.0</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="20" t="s">
         <v>1588</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="20" t="s">
         <v>1589</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="20" t="s">
         <v>19</v>
       </c>
       <c r="I14" s="17" t="s">
@@ -79841,7 +79894,7 @@
       <c r="C15" s="20" t="s">
         <v>1563</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="20">
         <v>14.0</v>
       </c>
       <c r="E15" s="20" t="s">
@@ -79867,16 +79920,16 @@
       <c r="B16" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="20" t="s">
         <v>1592</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="20">
         <v>15.0</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>1593</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="20" t="s">
         <v>1594</v>
       </c>
       <c r="H16" s="20" t="s">
@@ -79896,10 +79949,10 @@
       <c r="B17" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="20" t="s">
         <v>1592</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="20">
         <v>16.0</v>
       </c>
       <c r="E17" s="20" t="s">
@@ -79928,7 +79981,7 @@
       <c r="C18" s="20" t="s">
         <v>1592</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="20">
         <v>17.0</v>
       </c>
       <c r="E18" s="20" t="s">
@@ -79957,13 +80010,13 @@
       <c r="C19" s="20" t="s">
         <v>1592</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="20">
         <v>18.0</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>1599</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="20" t="s">
         <v>1600</v>
       </c>
       <c r="H19" s="20" t="s">
@@ -79986,7 +80039,7 @@
       <c r="C20" s="20" t="s">
         <v>1601</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="20">
         <v>19.0</v>
       </c>
       <c r="E20" s="20" t="s">
@@ -80015,13 +80068,13 @@
       <c r="C21" s="20" t="s">
         <v>1601</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="20">
         <v>20.0</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>1604</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="20" t="s">
         <v>1605</v>
       </c>
       <c r="H21" s="20" t="s">
@@ -80044,10 +80097,10 @@
       <c r="C22" s="20" t="s">
         <v>1601</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="20">
         <v>21.0</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="20" t="s">
         <v>1606</v>
       </c>
       <c r="G22" s="20" t="s">
@@ -80073,7 +80126,7 @@
       <c r="C23" s="20" t="s">
         <v>1601</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="20">
         <v>22.0</v>
       </c>
       <c r="E23" s="20" t="s">
@@ -80102,13 +80155,13 @@
       <c r="C24" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="20">
         <v>23.0</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>1611</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="20" t="s">
         <v>1612</v>
       </c>
       <c r="H24" s="20" t="s">
@@ -80131,13 +80184,13 @@
       <c r="C25" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="20">
         <v>24.0</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>1613</v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="G25" s="20" t="s">
         <v>1614</v>
       </c>
       <c r="H25" s="20" t="s">
@@ -80160,13 +80213,13 @@
       <c r="C26" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="20">
         <v>25.0</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>1615</v>
       </c>
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="26" t="s">
         <v>1616</v>
       </c>
       <c r="H26" s="20" t="s">
@@ -80189,13 +80242,13 @@
       <c r="C27" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="20">
         <v>26.0</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>1617</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="20" t="s">
         <v>1618</v>
       </c>
       <c r="H27" s="20">
@@ -80218,13 +80271,13 @@
       <c r="C28" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="20">
         <v>27.0</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="20" t="s">
         <v>1619</v>
       </c>
-      <c r="G28" s="26" t="s">
+      <c r="G28" s="20" t="s">
         <v>1620</v>
       </c>
       <c r="H28" s="20" t="s">
@@ -80247,10 +80300,10 @@
       <c r="C29" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="20">
         <v>28.0</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="20" t="s">
         <v>1621</v>
       </c>
       <c r="G29" s="20" t="s">
@@ -80276,13 +80329,13 @@
       <c r="C30" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="20">
         <v>29.0</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>1623</v>
       </c>
-      <c r="G30" s="26" t="s">
+      <c r="G30" s="20" t="s">
         <v>1624</v>
       </c>
       <c r="H30" s="20" t="s">
@@ -80305,13 +80358,13 @@
       <c r="C31" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="20">
         <v>30.0</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>1625</v>
       </c>
-      <c r="G31" s="26" t="s">
+      <c r="G31" s="20" t="s">
         <v>1626</v>
       </c>
       <c r="H31" s="20" t="s">
@@ -80334,7 +80387,7 @@
       <c r="C32" s="20" t="s">
         <v>1610</v>
       </c>
-      <c r="D32" s="26">
+      <c r="D32" s="20">
         <v>31.0</v>
       </c>
       <c r="E32" s="20" t="s">
@@ -80343,7 +80396,7 @@
       <c r="G32" s="20" t="s">
         <v>1628</v>
       </c>
-      <c r="H32" s="26" t="s">
+      <c r="H32" s="20" t="s">
         <v>37</v>
       </c>
       <c r="I32" s="17" t="s">
@@ -80360,16 +80413,16 @@
       <c r="B33" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="20" t="s">
         <v>1629</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="20">
         <v>32.0</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="20" t="s">
         <v>1630</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="27" t="s">
         <v>1631</v>
       </c>
       <c r="H33" s="20">
@@ -80383,12 +80436,33 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
+      <c r="A34" s="20" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>560</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>1629</v>
+      </c>
+      <c r="D34" s="20">
+        <v>33.0</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>1632</v>
+      </c>
+      <c r="G34" s="27" t="s">
+        <v>1633</v>
+      </c>
+      <c r="H34" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="17">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="20" t="s">
@@ -80397,11 +80471,20 @@
       <c r="B35" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="C35" s="26" t="s">
-        <v>1629</v>
-      </c>
-      <c r="D35" s="26">
-        <v>33.0</v>
+      <c r="C35" s="27" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D35" s="20">
+        <v>34.0</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>1635</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>1636</v>
+      </c>
+      <c r="H35" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="I35" s="17" t="s">
         <v>20</v>
@@ -80418,10 +80501,19 @@
         <v>560</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>1629</v>
-      </c>
-      <c r="D36" s="26">
-        <v>34.0</v>
+        <v>1634</v>
+      </c>
+      <c r="D36" s="20">
+        <v>35.0</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>1637</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>1638</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="I36" s="17" t="s">
         <v>20</v>
@@ -80437,8 +80529,20 @@
       <c r="B37" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D37" s="26">
-        <v>35.0</v>
+      <c r="C37" s="20" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D37" s="20">
+        <v>36.0</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>1639</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="I37" s="17" t="s">
         <v>20</v>
@@ -80454,8 +80558,20 @@
       <c r="B38" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D38" s="26">
-        <v>36.0</v>
+      <c r="C38" s="20" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D38" s="20">
+        <v>37.0</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>1641</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>1642</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="I38" s="17" t="s">
         <v>20</v>
@@ -80471,8 +80587,20 @@
       <c r="B39" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D39" s="26">
-        <v>37.0</v>
+      <c r="C39" s="20" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D39" s="20">
+        <v>38.0</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>1643</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H39" s="27" t="s">
+        <v>19</v>
       </c>
       <c r="I39" s="17" t="s">
         <v>20</v>
@@ -80488,8 +80616,20 @@
       <c r="B40" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D40" s="26">
-        <v>38.0</v>
+      <c r="C40" s="20" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D40" s="20">
+        <v>39.0</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>1645</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>1646</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="I40" s="17" t="s">
         <v>20</v>
@@ -80499,21 +80639,12 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="20" t="s">
-        <v>1562</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>560</v>
-      </c>
-      <c r="D41" s="26">
-        <v>39.0</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J41" s="17">
-        <v>1.0</v>
-      </c>
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
     </row>
     <row r="42">
       <c r="A42" s="20" t="s">
@@ -80522,7 +80653,7 @@
       <c r="B42" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D42" s="26">
+      <c r="D42" s="20">
         <v>40.0</v>
       </c>
       <c r="I42" s="17" t="s">
@@ -80539,7 +80670,7 @@
       <c r="B43" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D43" s="26">
+      <c r="D43" s="20">
         <v>41.0</v>
       </c>
       <c r="I43" s="17" t="s">
@@ -80556,7 +80687,7 @@
       <c r="B44" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D44" s="26">
+      <c r="D44" s="20">
         <v>42.0</v>
       </c>
       <c r="I44" s="17" t="s">
@@ -80573,7 +80704,7 @@
       <c r="B45" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D45" s="26">
+      <c r="D45" s="20">
         <v>43.0</v>
       </c>
       <c r="I45" s="17" t="s">
@@ -80590,7 +80721,7 @@
       <c r="B46" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D46" s="26">
+      <c r="D46" s="20">
         <v>44.0</v>
       </c>
       <c r="I46" s="17" t="s">
@@ -80607,7 +80738,7 @@
       <c r="B47" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D47" s="26">
+      <c r="D47" s="20">
         <v>45.0</v>
       </c>
       <c r="I47" s="17" t="s">
@@ -80624,7 +80755,7 @@
       <c r="B48" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D48" s="26">
+      <c r="D48" s="20">
         <v>46.0</v>
       </c>
       <c r="I48" s="17" t="s">
@@ -80641,7 +80772,7 @@
       <c r="B49" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D49" s="26">
+      <c r="D49" s="20">
         <v>47.0</v>
       </c>
       <c r="I49" s="17" t="s">
@@ -80658,7 +80789,7 @@
       <c r="B50" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D50" s="26">
+      <c r="D50" s="20">
         <v>48.0</v>
       </c>
       <c r="I50" s="17" t="s">
@@ -80675,7 +80806,7 @@
       <c r="B51" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D51" s="26">
+      <c r="D51" s="20">
         <v>49.0</v>
       </c>
       <c r="I51" s="17" t="s">
@@ -80692,7 +80823,7 @@
       <c r="B52" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D52" s="26">
+      <c r="D52" s="20">
         <v>50.0</v>
       </c>
       <c r="I52" s="17" t="s">
@@ -80709,7 +80840,7 @@
       <c r="B53" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D53" s="26">
+      <c r="D53" s="20">
         <v>51.0</v>
       </c>
       <c r="I53" s="17" t="s">
@@ -80726,7 +80857,7 @@
       <c r="B54" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D54" s="26">
+      <c r="D54" s="20">
         <v>52.0</v>
       </c>
       <c r="I54" s="17" t="s">
@@ -80743,7 +80874,7 @@
       <c r="B55" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D55" s="26">
+      <c r="D55" s="20">
         <v>53.0</v>
       </c>
       <c r="I55" s="17" t="s">
@@ -80760,7 +80891,7 @@
       <c r="B56" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D56" s="26">
+      <c r="D56" s="20">
         <v>54.0</v>
       </c>
       <c r="I56" s="17" t="s">
@@ -80777,7 +80908,7 @@
       <c r="B57" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D57" s="26">
+      <c r="D57" s="20">
         <v>55.0</v>
       </c>
       <c r="I57" s="17" t="s">
@@ -80794,7 +80925,7 @@
       <c r="B58" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D58" s="26">
+      <c r="D58" s="20">
         <v>56.0</v>
       </c>
       <c r="I58" s="17" t="s">
@@ -80811,7 +80942,7 @@
       <c r="B59" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D59" s="26">
+      <c r="D59" s="20">
         <v>57.0</v>
       </c>
       <c r="I59" s="17" t="s">
@@ -80828,7 +80959,7 @@
       <c r="B60" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D60" s="26">
+      <c r="D60" s="20">
         <v>58.0</v>
       </c>
       <c r="I60" s="17" t="s">
@@ -80845,7 +80976,7 @@
       <c r="B61" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D61" s="26">
+      <c r="D61" s="20">
         <v>59.0</v>
       </c>
       <c r="I61" s="17" t="s">
@@ -80862,7 +80993,7 @@
       <c r="B62" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D62" s="26">
+      <c r="D62" s="20">
         <v>60.0</v>
       </c>
       <c r="I62" s="17" t="s">
@@ -80879,7 +81010,7 @@
       <c r="B63" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D63" s="26">
+      <c r="D63" s="20">
         <v>61.0</v>
       </c>
       <c r="I63" s="17" t="s">
@@ -80896,7 +81027,7 @@
       <c r="B64" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D64" s="26">
+      <c r="D64" s="20">
         <v>62.0</v>
       </c>
       <c r="I64" s="17" t="s">
@@ -80910,7 +81041,7 @@
       <c r="B65" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D65" s="26">
+      <c r="D65" s="20">
         <v>63.0</v>
       </c>
       <c r="I65" s="17" t="s">
@@ -80924,7 +81055,7 @@
       <c r="B66" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D66" s="26">
+      <c r="D66" s="20">
         <v>64.0</v>
       </c>
       <c r="I66" s="17" t="s">
@@ -80938,7 +81069,7 @@
       <c r="B67" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D67" s="26">
+      <c r="D67" s="20">
         <v>65.0</v>
       </c>
       <c r="I67" s="17" t="s">
@@ -80952,7 +81083,7 @@
       <c r="B68" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D68" s="26">
+      <c r="D68" s="20">
         <v>66.0</v>
       </c>
       <c r="I68" s="17" t="s">
@@ -80966,7 +81097,7 @@
       <c r="B69" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D69" s="26">
+      <c r="D69" s="20">
         <v>67.0</v>
       </c>
       <c r="I69" s="22"/>
@@ -80978,7 +81109,7 @@
       <c r="B70" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D70" s="26">
+      <c r="D70" s="20">
         <v>68.0</v>
       </c>
       <c r="I70" s="22"/>
@@ -80990,7 +81121,7 @@
       <c r="B71" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D71" s="26">
+      <c r="D71" s="20">
         <v>69.0</v>
       </c>
       <c r="I71" s="22"/>
@@ -81002,7 +81133,7 @@
       <c r="B72" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D72" s="26">
+      <c r="D72" s="20">
         <v>70.0</v>
       </c>
       <c r="I72" s="22"/>
@@ -81014,7 +81145,7 @@
       <c r="B73" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D73" s="26">
+      <c r="D73" s="20">
         <v>71.0</v>
       </c>
       <c r="I73" s="22"/>
@@ -81026,7 +81157,7 @@
       <c r="B74" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D74" s="26">
+      <c r="D74" s="20">
         <v>72.0</v>
       </c>
       <c r="I74" s="22"/>
@@ -81038,7 +81169,7 @@
       <c r="B75" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D75" s="26">
+      <c r="D75" s="20">
         <v>73.0</v>
       </c>
       <c r="I75" s="22"/>
@@ -81050,7 +81181,7 @@
       <c r="B76" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D76" s="26">
+      <c r="D76" s="20">
         <v>74.0</v>
       </c>
       <c r="I76" s="22"/>
@@ -81062,7 +81193,7 @@
       <c r="B77" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D77" s="26">
+      <c r="D77" s="20">
         <v>75.0</v>
       </c>
       <c r="I77" s="22"/>
@@ -81074,7 +81205,7 @@
       <c r="B78" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D78" s="26">
+      <c r="D78" s="20">
         <v>76.0</v>
       </c>
       <c r="I78" s="22"/>
@@ -81086,7 +81217,7 @@
       <c r="B79" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D79" s="26">
+      <c r="D79" s="20">
         <v>77.0</v>
       </c>
       <c r="I79" s="22"/>
@@ -81098,7 +81229,7 @@
       <c r="B80" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D80" s="26">
+      <c r="D80" s="20">
         <v>78.0</v>
       </c>
       <c r="I80" s="22"/>
@@ -81110,7 +81241,7 @@
       <c r="B81" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D81" s="26">
+      <c r="D81" s="20">
         <v>79.0</v>
       </c>
       <c r="I81" s="22"/>
@@ -81122,7 +81253,7 @@
       <c r="B82" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D82" s="26">
+      <c r="D82" s="20">
         <v>80.0</v>
       </c>
       <c r="I82" s="22"/>
@@ -81131,7 +81262,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="D83" s="26">
+      <c r="D83" s="20">
         <v>81.0</v>
       </c>
       <c r="I83" s="22"/>
@@ -81140,7 +81271,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="D84" s="26">
+      <c r="D84" s="20">
         <v>82.0</v>
       </c>
       <c r="I84" s="22"/>
@@ -84427,7 +84558,7 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>1632</v>
+        <v>1647</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>281</v>
@@ -84438,7 +84569,7 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>1633</v>
+        <v>1648</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>39</v>
@@ -84449,7 +84580,7 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>1634</v>
+        <v>1649</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>262</v>

</xml_diff>